<commit_message>
updates to test data
</commit_message>
<xml_diff>
--- a/testdata/xlsx/01.01-general.xlsx
+++ b/testdata/xlsx/01.01-general.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F3F44941-D809-4BC5-903B-0A59A274BC75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{05933C7B-3502-4541-9372-7300D458CAA6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="10425" tabRatio="341" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,12 +596,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>international</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -638,9 +632,6 @@
     <t>separator</t>
   </si>
   <si>
-    <t>brack</t>
-  </si>
-  <si>
     <t>escape</t>
   </si>
   <si>
@@ -789,6 +780,15 @@
   </si>
   <si>
     <t xml:space="preserve">  2001-12-25 01:02:03</t>
+  </si>
+  <si>
+    <t>ascii</t>
+  </si>
+  <si>
+    <t>unicode</t>
+  </si>
+  <si>
+    <t>bracket</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1654,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1667,7 +1667,7 @@
     <col min="12" max="12" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
@@ -1684,67 +1684,67 @@
         <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>147</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1800,13 +1800,13 @@
         <v>75</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>31</v>
@@ -1865,22 +1865,22 @@
         <v>85</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1933,19 +1933,19 @@
         <v>78</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2001,10 +2001,10 @@
         <v>74</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>34</v>
@@ -2060,16 +2060,16 @@
         <v>79</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>180</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>34</v>
@@ -2083,7 +2083,7 @@
         <v>150</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>160</v>
@@ -2128,10 +2128,10 @@
         <v>80</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>112</v>
@@ -2140,7 +2140,7 @@
         <v>34</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2193,16 +2193,16 @@
         <v>144</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>31</v>
@@ -2261,16 +2261,16 @@
         <v>82</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>31</v>
@@ -2329,16 +2329,16 @@
         <v>81</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>31</v>
@@ -2397,16 +2397,16 @@
         <v>84</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>31</v>
@@ -2465,16 +2465,16 @@
         <v>83</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>34</v>
@@ -2533,16 +2533,16 @@
         <v>87</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>34</v>

</xml_diff>